<commit_message>
eerste iteratie gedaan 2de staat klaar voor te labelen
</commit_message>
<xml_diff>
--- a/Identifier/to_label.xlsx
+++ b/Identifier/to_label.xlsx
@@ -458,3201 +458,3201 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hoe verhouden de cijfers zich tot het Vlaamse gemiddelde?</t>
+          <t>Is er een positieve trend waar te nemen en zo ja, welke?</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5178589820861816</v>
+        <v>0.5608973503112793</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4821410179138184</v>
+        <v>0.4391026496887207</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Heeft de minister het doel om 100.000 bomen te planten in de Vlaamse Rand vanaf 2022 gehaald?</t>
+          <t>2021 2022Antwerpen 274 415Limburg 23 44Oost-Vlaanderen 121 195Vlaams-Brabant 58 85West-Vlaanderen 59 92Daarnaast geeft onderstaande tabel weer hoeveel e-stepslachtoffers er vielen in die ongevallen, opgedeeld naar provincie en letselernst (bron: FOD Economie, Statbel).</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5639283061027527</v>
+        <v>0.5643495321273804</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4360716938972473</v>
+        <v>0.4356504678726196</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Verwacht hij dat het aantal leerlingen in het buitengewoon onderwijs de komende jaren zal afnemen?</t>
+          <t>214 kreeg ik volgende tabel van de minister voor het jaar 2018:Hoe wordt het PVB ingezet in 2018?% onderbenutting Aantal personenEnkel via voucher 0,95 % 21.015Enkel via cash nVZA 19,74 % 1.784Enkel via cash VZA 6,87 % 53Voucher en cash nVZA 12,37 % 1.056Voucher en cash VZA 4,03 % 41Cash VZA en cash nVZA 13,61 % 313Voucher, cash VZA en cash nVZA 11,90 % 158(nog) geen besteding cash of voucher99,35 % 323Allen 3,50 % 24.420Kan de minister een update van die tabel bezorgen voor de jaren 2019, 2020 en 2021?</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5670823454856873</v>
+        <v>0.5681431293487549</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4329176545143127</v>
+        <v>0.4318568706512451</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>817 gaf de minister aan dat de resultaten Kan de minister een cijfermatige en beoordelende update geven van de effecten van de uitbreiding van het verlof voor verminderde prestaties wegens ziekte voor de personeelsleden van de hogescholen?</t>
+          <t>Wanneer is die aanvraag ingediend?</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5842055678367615</v>
+        <v>0.5681633353233337</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4157944321632385</v>
+        <v>0.4318366646766663</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Als het effectief om een besparing gaat, zoals de cijfers lijken aan te tonen, is het dan al duidelijk waar het geld concreet bespaard zal worden?</t>
+          <t>Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5856462121009827</v>
+        <v>0.5703068375587463</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4143537878990173</v>
+        <v>0.4296931624412537</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Heeft de minister er zicht op hoe dat bedrag concreet werd geïnvesteerd?</t>
+          <t>Hoe evalueert de minister de cijfers ten opzichte van voorgaande jaren?</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5861800909042358</v>
+        <v>0.5949475169181824</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4138199090957642</v>
+        <v>0.4050524830818176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Wat is voor de zwarte verkeerspunten in West-Vlaanderen die (nog) op de lijst staan:a) de stand van zaken;b) de timing om ze aan te pakken;c) het vermoedelijke budget;d) de eventueel betrokken partners?</t>
+          <t>Wat zijn de verschillen van onderbenutting wanneer het PVB is verkregen via de reguliere procedure of via de automatische toekenningsgroepen (opgedeeld per automatische toekenningsgroep)?</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5889269113540649</v>
+        <v>0.5978026986122131</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4110730886459351</v>
+        <v>0.4021973013877869</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Zal hij ze allemaal planten tegen het einde van de legislatuur?</t>
+          <t>Wanneer is het proces-verbaal door het Departement Omgeving opgemaakt?</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5975625514984131</v>
+        <v>0.6018190979957581</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4024374485015869</v>
+        <v>0.3981809020042419</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Wie in een Limburgse risicozone een wolf-werende omheining plaatst, kan vanuit ANB rekenen op zowel een plaatsings-, als een onderhoudsvergoeding.</t>
+          <t>Welk aandeel van de kruispunten in Vlaanderen, beheerd door het Agentschap Wegen en Verkeer (AWV), is intussen conflictvrij?</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6313496828079224</v>
+        <v>0.6179395318031311</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3686503171920776</v>
+        <v>0.3820604681968689</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kan de minister een overzicht bezorgen van de Vlaamse gemeenten die een samenwerkingsakkoord onderhielden met Dyzo?</t>
+          <t>Worden er veel afwijkingen vastgesteld op de tweejaarlijkse ijking?</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6439708471298218</v>
+        <v>0.6183764338493347</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3560291528701782</v>
+        <v>0.3816235661506653</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Heeft de VRM toegezegd dat de omschakeling naar Nostalie Plus voldoende is om de erkenning te behouden?</t>
+          <t>Hoe evalueert de minister deze cijfers?</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6529092192649841</v>
+        <v>0.624126136302948</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3470907807350159</v>
+        <v>0.375873863697052</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Indien de minister een aanpassing plant, wat is daarvan het concept, de timing en het budget?</t>
+          <t>Hoe evalueert de minister deze cijfers?</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6654695272445679</v>
+        <v>0.624126136302948</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3345304727554321</v>
+        <v>0.375873863697052</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021-2022 2022-2023Provincie# ingeschreven lln in 1B#lln die het LO niet afwerkten %# ingeschreven lln in 1B#lln die het LO niet afwerkten%Antwerpen 3.047 52117,10% 3.164 464 14,66%Brussels Hoofdstedelijk Gewest 361 6818,84% 363 48 13,22%Limburg 1.398 31122,25% 1.419 299 21,07%Oost-Vlaanderen 2.365 32613,78% 2.581 454 17,59%Vlaams-Brabant 1.199 23519,60% 1.311 204 15,56%West-Vlaanderen 1.664 22613,58% 1.801 272 15,10%Totaal 10.034 1.68716,81% 10.639 1.741 16,36%Onderstaande tabel geeft weer hoeveel leerlingen de voorbije 2 schooljaren tijdens het schooljaar doorstroomden van 1A naar 1B met gunstige beslissing van de toelatingsklassenraad.</t>
+          <t>Hoe evalueert de minister deze cijfers?</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6741490364074707</v>
+        <v>0.624126136302948</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3258509635925293</v>
+        <v>0.375873863697052</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>57 (2023-2024) over de werking en veiligheid van de dierenartsen met opdracht in de slachthuizen, stelde de minister dat momenteel 56 DMO’s een contract met de Vlaamse overheid hebben, van wie er 46 een vaste opdracht uitvoeren.</t>
+          <t>Hoe evalueert de minister deze cijfers?</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6788867712020874</v>
+        <v>0.624126136302948</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3211132287979126</v>
+        <v>0.375873863697052</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kunnen de cijfers ook voor die instellingen gegeven worden?</t>
+          <t>Hoe evalueert de minister deze cijfers?</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.682645320892334</v>
+        <v>0.624126136302948</v>
       </c>
       <c r="D16" t="n">
-        <v>0.317354679107666</v>
+        <v>0.375873863697052</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bijvoorbeeld een maximale geluidsnorm voor niet-ingedeelde warmtepompen van 40 dB op de perceelsgrens? Zo ja, wat zijn de stappen die de minister daarvoor gaat ondernemen en wat is de vooropgestelde timing?</t>
+          <t>&gt; 60 jaar?</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6953750252723694</v>
+        <v>0.6513121724128723</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3046249747276306</v>
+        <v>0.3486878275871277</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Welke timing plant de minister voor de uit dit besluit voortkomende beautycontest?</t>
+          <t>&gt; 60 jaar?</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7019119262695312</v>
+        <v>0.6513121724128723</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2980880737304688</v>
+        <v>0.3486878275871277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kan de minister de meest recente dynamische lijst beschikbaar stellen van de provincie West-Vlaanderen?</t>
+          <t>&gt; 60 jaar?</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7160115242004395</v>
+        <v>0.6513121724128723</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2839884757995605</v>
+        <v>0.3486878275871277</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Kan de minister toelichten of de initiatieven van de pleegzorggemeenten merkbare positieve effecten hebben gehad; hebben er het afgelopen jaar bijvoorbeeld meer gezinnen zich aangemeld als pleeggezin ten opzichte van de vorige jaren?</t>
+          <t>&gt; 60 jaar?</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7251467704772949</v>
+        <v>0.6513121724128723</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2748532295227051</v>
+        <v>0.3486878275871277</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>d) Waarom voorziet ANB nog in de aanwerving van vier bijkomende “everzwijnspecialisten met jachtverlof” ter aanvulling/ondersteuning van de al aangestelde Vlaamse everzwijncoördinator?</t>
+          <t>De gegevens voor 2022 worden momenteel verwerkt zodat ook deze ter beschikking kunnen worden gesteld via het Dataplatform Departement Werk en Sociale Economie ( Open data | Vlaanderen.be)a-b) Overzicht van het aantal maatwerkbedrijven, opgedeeld naar hoeveel maatwerkers er actief zijn binnen de onderneming en contingent2022 - Totaal 126 126 126 124 122 122Toegekend contingent19.740 19.740 19.740 20.014 20.082 20.082Het aantal maatwerkbedrijven daalt over de kwartalen heen, omwille van een fusiebeweging binnen de sector die in 2021 is ingezet en zich nog steeds verderzet.</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7296812534332275</v>
+        <v>0.6526496410369873</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2703187465667725</v>
+        <v>0.3473503589630127</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Welke extra subsidies verleent de minister aan de scholen en onderwijsinstellingen om leerlingen die gevlucht zijn uit Oekraïne op te vangen?</t>
+          <t>Vanaf wanneer is de geboden ondersteuning niet voldoende aangepast?</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7450641393661499</v>
+        <v>0.6855155229568481</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2549358606338501</v>
+        <v>0.3144844770431519</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Wie in Limburg echter een everzwijn-werende omheining of elektrische draad plaatst die vereist is om in aanmerking te kunnen komen voor de vergoeding van everzwijnschade, moet zelf voor deze kosten opdraaien.</t>
+          <t>Welke van die dossiers staan al op het meerjaren-GIP en voor welk bedrag per jaar?</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7459707856178284</v>
+        <v>0.6889446377754211</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2540292143821716</v>
+        <v>0.3110553622245789</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Heeft de VRM eraan herinnerd dat men 70% muziek van de laatste vijf jaar moet draaien conform het ingediende dossier?</t>
+          <t>Deze manier van evalueren laat toe te achterhalen hoeveel bestuurders zich de campagne na afloop kunnen herinneren (bereik) en wat het effect autobestuurder.</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7493088245391846</v>
+        <v>0.7051619291305542</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2506911754608154</v>
+        <v>0.2948380708694458</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Is het een optie om de beheersovereenkomsten met herders uit te breiden van bijvoorbeeld twee naar vijf graasbeurten?</t>
+          <t>Of dat lukt, zal vooral afhangen van het aantal mensen dat een ticket individueel maatwerk krijgt en van hoeveel bedrijven de inspanning willen doen om personen met zo’n ticket tewerk te stellen.</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7543051242828369</v>
+        <v>0.705502450466156</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2456948757171631</v>
+        <v>0.294497549533844</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Is ondertussen de exacte datum voor de Contract Close gekend? Zo ja, wat is de exacte datum?</t>
+          <t>Zijn er in de nabije toekomst nog bijkomende initiatieven gepland om studenten met een handicap of functiebeperking te ondersteunen? Zo ja, wat is het plan van aanpak en het budget?</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7698290944099426</v>
+        <v>0.7127206325531006</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2301709055900574</v>
+        <v>0.2872793674468994</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Hoe evolueerden de aantallen hierboven de voorbije 3 jaar?</t>
+          <t>Zijn er in de nabije toekomst nog bijkomende initiatieven gepland om studenten met een handicap of functiebeperking te ondersteunen? Zo ja, wat is het plan van aanpak en het budget?</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0.770662784576416</v>
+        <v>0.7127206325531006</v>
       </c>
       <c r="D27" t="n">
-        <v>0.229337215423584</v>
+        <v>0.2872793674468994</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>c) Wat waren de resultaten van de vooronderzoeken en stabiliteitsstudie die al werden opgestart?</t>
+          <t>Wanneer zal de derde oproep door de Vlaamse Regering in de markt worden gezet?</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7716574668884277</v>
+        <v>0.7300378680229187</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2283425331115723</v>
+        <v>0.2699621319770813</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>c) Kan de minister een overzicht geven van het ondersteuningsaanbod per casus?</t>
+          <t>Hoe evolueert het aantal aanvragen en goedkeuringen in het kader van de projectoproep Landbouw - Natuur doorheen de jaren?</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7771450877189636</v>
+        <v>0.7364243865013123</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2228549122810364</v>
+        <v>0.2635756134986877</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Werd de omgevingsvergunning afgeleverd?</t>
+          <t>c) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7787595391273499</v>
+        <v>0.7377975583076477</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2212404608726501</v>
+        <v>0.2622024416923523</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kan de minister een lijst van de getraceerde ‘grijze punten’ geven?</t>
+          <t>c) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7909579277038574</v>
+        <v>0.7377975583076477</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2090420722961426</v>
+        <v>0.2622024416923523</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Op zijn website stelt ANB: “een aantal A1-studies in landen die al langer met deze invasieve exoot te maken hebben, wijzen erop dat de schade aan de honingbij onmiskenbaar is [3].” Beschikt de minister ook al over eigen Vlaamse cijfergegevens voor de jaren 2019, 2020, 2021, 2022 en 2023 wat betreft enerzijds het aantal door de Vlaamse imkers geregistreerde bijenkasten/bijenvolken in Vlaanderen en anderzijds het aantal bijenkasten/bijenvolken dat tijdens voormelde jaren door de Aziatische hoornaar werd uitgemoord? Zo ja, graag een schematisch overzicht van deze data?</t>
+          <t>c) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7925609946250916</v>
+        <v>0.7377975583076477</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2074390053749084</v>
+        <v>0.2622024416923523</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Hoelang duurde die ontkoppeling gemiddeld?</t>
+          <t>c) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.7967144250869751</v>
+        <v>0.7377975583076477</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2032855749130249</v>
+        <v>0.2622024416923523</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Wie in de buurt van een nest komt, riskeert immers een massale aanval van Aziatische hoornaars, en met het exponentieel toenemend aantal nesten neemt dat risico in Vlaanderen alleen maar evenredig toe.</t>
+          <t>Is het ziekteverzuim bij De Lijn gestegen sinds het ziektebriefje voor 1 dag is afgeschaft?</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7974569797515869</v>
+        <v>0.7395509481430054</v>
       </c>
       <c r="D34" t="n">
-        <v>0.2025430202484131</v>
+        <v>0.2604490518569946</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Over welke cijfers beschikt de administratie van de minister met betrekking tot Indiase verpleegkundigen?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7985000610351562</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2014999389648438</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>De minister laat weten dat de hogescholen vrij zijn om te bepalen hoeveel graduaatsopleidingen ze wensen in te richten, maar dat ze er ook moeten over waken dat die opleidingen op lange termijn door de instellingen gefinancierd kunnen worden.</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8024354577064514</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1975645422935486</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Het basisonderwijs is, zoals het woord het zegt, het onderwijssegment waar aan leerlingen de basis van alle schoolse leerstof wordt geleerd; als we dan als overheid in een kaderdecreet vastleggen dat de basis bestaat uit zestien sleutelcompetenties, dan is het toch tegenstrijdig dat er sleutelcompetenties leeg worden gelaten?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8070237040519714</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1929762959480286</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>b) Plant de minister om nieuwe/andere subsidies of extra middelen te verlenen aan scholen/onderwijsinstellingen in het kader van de opvang van leerlingen uit Oekraïne in het schooljaar 2023-2024?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>0.814944326877594</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D38" t="n">
-        <v>0.185055673122406</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Leerlingen die niet uit het hoofd kunnen uitrekenen hoeveel 18+13 is, die geen analoge klok kunnen lezen, die basiswoorden niet begrijpen, laat staan dat ze die correct kunnen schrijven, etc.</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0.817829966545105</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D39" t="n">
-        <v>0.182170033454895</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Liggen alle 874 schoolrouteknelpunten op gewestelijke infrastructuur, of is er ook sprake van schoolrouteknelpunten op lokale wegen die met die middelen aangepakt worden?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0.8197145462036133</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1802854537963867</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bij het overhevelen van de graduaatsopleidingen van de centra voor volwassenenonderwijs (CVO’s) naar de hogescholen in 2019, wijzigde de financiering Werd bij die beslissing rekening gehouden met het mogelijke succes van die opleidingen, waardoor het aantal opgenomen studiepunten significant veel groter is dan de aanpassing van de financiering (aantal inschrijvingen 2022-2023: +16%; stijging financiering: +2%)?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.8207924365997314</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D41" t="n">
-        <v>0.1792075634002686</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://extranet.vaph.be/jaarverslag/2022/pages/25/ voor 2022 en via https://www.vaph.be/documenten?f%5B0%5D=type%3A54 voor de voorafgaande jaren.</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8212417364120483</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1787582635879517</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Zal het pakket bijdragen aan het halen van de STEM-leerdoelen, zoals de uitgeverij beweert?</t>
+          <t>Werden die maatregelen geëvalueerd en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8215951323509216</v>
+        <v>0.7468575239181519</v>
       </c>
       <c r="D43" t="n">
-        <v>0.1784048676490784</v>
+        <v>0.2531424760818481</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Zijn er voldoende reserveonderdelen en technici om de lift bij problemen onmiddellijk te herstellen?</t>
+          <t>Uit welke steun bestaat deze 14,2 miljoen euro?</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8236657381057739</v>
+        <v>0.782109260559082</v>
       </c>
       <c r="D44" t="n">
-        <v>0.1763342618942261</v>
+        <v>0.217890739440918</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Hoe verklaart de minister dat zoveel adviserende gemeenten de nochtans al vorig jaar aangevraagde adviezen nog niet hebben afgeleverd?</t>
+          <t>Is de minister tevreden over het aantal toegekende subsidies en de effecten van de oproep?</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8240914940834045</v>
+        <v>0.788632869720459</v>
       </c>
       <c r="D45" t="n">
-        <v>0.1759085059165955</v>
+        <v>0.211367130279541</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Toch prijkt onder de lijst van 2021 van degenen aan wie zo’n ereteken werd toegekend Pfizer Belgium, niet meteen een natuurlijke persoon.</t>
+          <t>Is de minister tevreden over het aantal toegekende subsidies en de effecten van de oproep?</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.825647234916687</v>
+        <v>0.788632869720459</v>
       </c>
       <c r="D46" t="n">
-        <v>0.174352765083313</v>
+        <v>0.211367130279541</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Kan een overzicht gegeven worden van de financiering van dit project?</t>
+          <t>Kan de minister een overzicht geven van alle lokale dienstencentra in Vlaanderen?</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>0.8267066478729248</v>
+        <v>0.7890015840530396</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1732933521270752</v>
+        <v>0.2109984159469604</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Kan de minister een overzicht geven van de gemeenten die momenteel niet over een volledige gemeenteraad beschikken?</t>
+          <t>Zal de minister deze legislatuur nog budgetten reserveren voor de stelplaatsen in Antwerpen, behalve de reguliere budgetten voor onderhoud en werking?</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8310822248458862</v>
+        <v>0.7975480556488037</v>
       </c>
       <c r="D48" t="n">
-        <v>0.1689177751541138</v>
+        <v>0.2024519443511963</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Was in die sterke groei voorzien?</t>
+          <t>Plant de minister initiatieven om deze anomalie recht te zetten? Zo ja, welke en wanneer kunnen we dat verwachten?</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8522295355796814</v>
+        <v>0.8293402194976807</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1477704644203186</v>
+        <v>0.1706597805023193</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>f) Hoelang duurt het gemiddeld vooraleer een vacature wordt ingevuld?</t>
+          <t>Hoe evalueert de minister de cijfers?</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>0.858546257019043</v>
+        <v>0.8312382698059082</v>
       </c>
       <c r="D50" t="n">
-        <v>0.141453742980957</v>
+        <v>0.1687617301940918</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Kan de minister een overzicht van de kansarmoede-index voor de gemeente Zoutleeuw geven en daarbij de collectieve opvangfaciliteit van Fedasil buiten beschouwing laten?</t>
+          <t>b) Wanneer zijn deze toestemmingen/documenten aangevraagd?</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8586463928222656</v>
+        <v>0.831916868686676</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1413536071777344</v>
+        <v>0.168083131313324</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Wie het centenboekje van de Vlaamse Regering van iets dichter bekijkt, ziet echter dat er naast de 4 miljoen euro extra voor jeugdinfrastructuur, ook een besparing van 5 miljoen euro op jeugdinfrastructuur wordt doorgevoerd.</t>
+          <t>Provincie Indiener Project Totaal projectbedrag (euro)Komt in aanmerking voor subsidiëring?</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8626709580421448</v>
+        <v>0.8368119597434998</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1373290419578552</v>
+        <v>0.1631880402565002</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Valt een dergelijk pakket te rijmen met de objectieven rond educatie voor duurzame ontwikkeling?</t>
+          <t>Welke eindbestemming werd er voor elke grond gevonden?</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8629118800163269</v>
+        <v>0.8370885848999023</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1370881199836731</v>
+        <v>0.1629114151000977</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Zo niet, wat plant de minister te doen met het eventuele resterende budget?</t>
+          <t>b) Kan de minister een lijst geven - ingedeeld naar provincie en naar gemeente of stad - van alle kruispunten die momenteel op de lijst van zwarte kruispunten staan?</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>0.8665314912796021</v>
+        <v>0.8371675610542297</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1334685087203979</v>
+        <v>0.1628324389457703</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Kan de minister de haalbaarheidsstudie bezorgen?</t>
+          <t>werd de studie betaald met het voorbehouden budget van 700.000 euro van toenmalig bevoegd minister Weyts in 2017?</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.87314373254776</v>
+        <v>0.8462185859680176</v>
       </c>
       <c r="D55" t="n">
-        <v>0.12685626745224</v>
+        <v>0.1537814140319824</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Met andere woorden: welke zaken waar eerst middelen voor begroot waren, zullen nu niet uitgevoerd kunnen worden als gevolg van de besparing?</t>
+          <t>Welke voorwaarden rond tewerkstelling zijn er gekoppeld aan deze steun en wat zijn de termijnen die men moet naleven?</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.8911840915679932</v>
+        <v>0.8467148542404175</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1088159084320068</v>
+        <v>0.1532851457595825</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>De minister gaf aan dat het nog te vroeg was om gedetailleerde cijfers over de invulling VDAB wel kan meedelen hoeveel werkzoekenden al werden toegeleid naar de gemeenschapsdienst.</t>
+          <t>Vanaf wanneer zal de maatregel ingaan?</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8962787389755249</v>
+        <v>0.8472135663032532</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1037212610244751</v>
+        <v>0.1527864336967468</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>- Wat is de impact van deze gebruiksduur op de bestaande levenspaden van manuele rolstoelen?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem stappen en timing hierin worden vooropgesteld en hoeveel het budget bedraagt?</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8970368504524231</v>
+        <v>0.8501444458961487</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1029631495475769</v>
+        <v>0.1498555541038513</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>a) Kan dat inderdaad afgeleid worden uit de cijfers van het aantal vastgestelde overtredingen?</t>
+          <t>Komen die gronden ook voor in de cijfers op de slide van de presentatie?</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>0.901175856590271</v>
+        <v>0.8548300266265869</v>
       </c>
       <c r="D59" t="n">
-        <v>0.098824143409729</v>
+        <v>0.1451699733734131</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Wat zal de exacte aard zijn van de minimumdoelen Nederlands voor kleuters?</t>
+          <t>Welke timing zal daarbij gehanteerd worden?</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>0.902548611164093</v>
+        <v>0.8606788516044617</v>
       </c>
       <c r="D60" t="n">
-        <v>0.09745138883590698</v>
+        <v>0.1393211483955383</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Kan hij daarnaast een opdeling geven, in totaal en per casus, waarbij de verbindingsofficieren ofwel vóór ofwel na de publieke aankondiging van het nieuwe asielcentrum werden betrokken?</t>
+          <t>Wat was de kostprijs van deze studie en waarom moet er door datzelfde studiebureau opnieuw bijkomend onderzoek worden gedaan naar de kilometerheffing?</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9148707389831543</v>
+        <v>0.861691415309906</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0851292610168457</v>
+        <v>0.138308584690094</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Kan de minister een opdeling geven van deze personen per snel degeneratieve aandoening voor 2021 en 2022?</t>
+          <t>d) Zal er elders voldoende stelplaatscapaciteit beschikbaar zijn om dat op te vangen?</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9217867851257324</v>
+        <v>0.8657521605491638</v>
       </c>
       <c r="D62" t="n">
-        <v>0.07821321487426758</v>
+        <v>0.1342478394508362</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>a) Wat is het effect van een fusie op enerzijds het tarief en anderzijds de werkelijke waarde van een opcentiem?</t>
+          <t>b) Wanneer loopt deze aanvraagperiode dan af?</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.922995924949646</v>
+        <v>0.866767406463623</v>
       </c>
       <c r="D63" t="n">
-        <v>0.077004075050354</v>
+        <v>0.133232593536377</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Zijn er export- en importcijfers beschikbaar?</t>
+          <t>Als er grote verschillen zijn in het aantal aanvragen per provincie, hoe verklaart de minister dan die verschillen?</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9237696528434753</v>
+        <v>0.86737060546875</v>
       </c>
       <c r="D64" t="n">
-        <v>0.07623034715652466</v>
+        <v>0.13262939453125</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>a) Betekent dit dat die 112 trajecten voor klanten die langer dan twee jaar werkzoekend zijn per definitie trajecten in de gemeenschapsdienst zullen worden?</t>
+          <t>Als er grote verschillen zijn in het aantal aanvragen per provincie, hoe verklaart de minister dan die verschillen?</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>0.923859179019928</v>
+        <v>0.86737060546875</v>
       </c>
       <c r="D65" t="n">
-        <v>0.07614082098007202</v>
+        <v>0.13262939453125</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Indien voor het bovenstaande geen cijfers beschikbaar zijn, is het dan zinvol om de cijfers in de toekomst te verzamelen?</t>
+          <t>a) Zullen de rijexamencentra voorzien worden van extra middelen om die toestellen b) Heeft deze nieuwe regelgeving een financiële impact op de kostprijs van het rijexamen voor de kandidaat-bestuurder? Zo ja, welke?</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9247907996177673</v>
+        <v>0.8768247961997986</v>
       </c>
       <c r="D66" t="n">
-        <v>0.07520920038223267</v>
+        <v>0.1231752038002014</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Welke budgetten moeten nog uitgetrokken worden voor de knelpunten die nog uitgevoerd moeten worden?</t>
+          <t>De gegevens voor 2022 worden momenteel verwerkt zodat ook deze ter beschikking kunnen worden gesteld via het Dataplatform Departement Werk en Sociale Economie ( Open data | Vlaanderen.be)a-b) Overzicht van het aantal LDE-ondernemingen, opgedeeld naar hoeveel LDE’ers er actief zijn binnen de onderneming (ondernemingen met minder dan 5, 5-10, 11-20, 21-50, 51-100, 100+) en contingent.</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>0.927467405796051</v>
+        <v>0.8771883249282837</v>
       </c>
       <c r="D67" t="n">
-        <v>0.07253259420394897</v>
+        <v>0.1228116750717163</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Wat is zijn de budgettaire implicaties van dat nieuwe statuut?</t>
+          <t>Wanneer werd de opdracht van het studiebureau Tractebel Engineering nv afgerond?</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9276491403579712</v>
+        <v>0.878750741481781</v>
       </c>
       <c r="D68" t="n">
-        <v>0.07235085964202881</v>
+        <v>0.121249258518219</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Wat betekent die overgangsregeling met betrekking tot de ontslagregeling concreet?</t>
+          <t>Kan de minister meedelen telkens voor het jaar 2021, 2022 en 2023?</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9329578876495361</v>
+        <v>0.8887544274330139</v>
       </c>
       <c r="D69" t="n">
-        <v>0.06704211235046387</v>
+        <v>0.1112455725669861</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Zijn de scholen vragende partij om het maximale aantal dagen per leerling op te trekken?</t>
+          <t>Kan de minister een oplijsting bezorgen van de West-Vlaamse scholen en verenigingen die deelnamen in het schooljaar 2022-2023, met vermelding van de gemeente waarbinnen de school of vereniging gevestigd is, de status van het actieplan (al dan niet voltooid) en de toegekende beloning per school en per vereniging?</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>0.9344092607498169</v>
+        <v>0.8907580375671387</v>
       </c>
       <c r="D70" t="n">
-        <v>0.06559073925018311</v>
+        <v>0.1092419624328613</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Wie geregeld gaat wandelen en fietsen, kan er niet meer naast kijken: de Japanse duizendknoop duikt overal, gaande van dijken over natuurgebieden tot zelfs ‘reguliere’ velden, op en overwoekert zo de bestaande gewassen en grassen.</t>
+          <t>a) Is de minister tevreden over het aantal aanvragen?</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.936144232749939</v>
+        <v>0.8973835706710815</v>
       </c>
       <c r="D71" t="n">
-        <v>0.06385576725006104</v>
+        <v>0.1026164293289185</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Er is vanuit het onderwijs een nieuw systeem ontwikkeld - de Movis-apps - waarmee de scholen de leerlingen inschrijven en waarin ook in aangeduid wordt wie gebruik wenst te maken van het leerlingenvervoer.</t>
+          <t>Wanneer is dat voor het laatst gemeten?</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9379714727401733</v>
+        <v>0.8974357843399048</v>
       </c>
       <c r="D72" t="n">
-        <v>0.06202852725982666</v>
+        <v>0.1025642156600952</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Hoe evolueren voorgaande cijfers bij fusionerende gemeenten?</t>
+          <t>Kan de minister een overzicht geven van de schoolroutes in Limburg waar verkeersslachtoffers bij 6- tot 18-jarigen vielen in de laatste vijf jaar?</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73" t="n">
-        <v>0.9383770823478699</v>
+        <v>0.9072400331497192</v>
       </c>
       <c r="D73" t="n">
-        <v>0.06162291765213013</v>
+        <v>0.09275996685028076</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Het is vaak een reminder of trigger voor al wie misschien al interesse heeft, maar nog twijfelt.</t>
+          <t>Welke timing wordt voor het volledige project gehanteerd?</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9424065947532654</v>
+        <v>0.9150487780570984</v>
       </c>
       <c r="D74" t="n">
-        <v>0.05759340524673462</v>
+        <v>0.08495122194290161</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Heeft de minister er zicht op of de extra middelen voldoende kostendekkend zijn om de vooropgestelde doelen te bereiken?</t>
+          <t>Kunnen de cijfers van de diversiteitsonderzoeken van 2021 en 2022 bekendgemaakt worden, aangezien ze aanwezig blijken?</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>0.94249427318573</v>
+        <v>0.9174978733062744</v>
       </c>
       <c r="D75" t="n">
-        <v>0.05750572681427002</v>
+        <v>0.08250212669372559</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Hoe dan?" met daarin propaganda voor een groot auto-infrastructuurproject gefinancierd met Vlaams belastinggeld.</t>
+          <t>Hoe breed is het tweerichtingsfietspad langs de Lierselei?</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9431845545768738</v>
+        <v>0.9182776808738708</v>
       </c>
       <c r="D76" t="n">
-        <v>0.05681544542312622</v>
+        <v>0.08172231912612915</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Hoe realistisch is het blijven aanhouden van alle 16 sleutelcompetenties zonder dat bepaalde sleutelcompetenties worden gereduceerd tot restjescompetenties?</t>
+          <t>Waren er in het schooljaar 2021-2022 tekorten aan leerwerkplekken?</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9465851187705994</v>
+        <v>0.918756902217865</v>
       </c>
       <c r="D77" t="n">
-        <v>0.05341488122940063</v>
+        <v>0.08124309778213501</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Kan per provincie een concreet overzicht gegeven worden van welke projecten dit jaar uitgevoerd kunnen/konden worden met het vooropgestelde budget van 15 miljoen euro?</t>
+          <t>b) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9518905878067017</v>
+        <v>0.9215774536132812</v>
       </c>
       <c r="D78" t="n">
-        <v>0.04810941219329834</v>
+        <v>0.07842254638671875</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>c) Wat voor type warmtebron betreft het?</t>
+          <t>b) Hoe evalueert de minister die cijfers?</t>
         </is>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.952265739440918</v>
+        <v>0.9215774536132812</v>
       </c>
       <c r="D79" t="n">
-        <v>0.04773426055908203</v>
+        <v>0.07842254638671875</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Kan de minister al evalueren of er voldoende budget is vrijgemaakt om de werken zo snel mogelijk uit te voeren?</t>
+          <t>Hoe is de verhouding in bekeuringen van Belgische ten opzichte van buitenlandse vrachtvervoerders?</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>1</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9538945555686951</v>
+        <v>0.9217989444732666</v>
       </c>
       <c r="D80" t="n">
-        <v>0.04610544443130493</v>
+        <v>0.0782010555267334</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Moet men in lerarenopleidingen secundair onderwijs bijvoorbeeld meer inzetten op kruisbestuiving met de lerarenopleiding lager onderwijs, aangezien het niveau van de leerlingen vaak ook dat van een lagereschoolleerling is?</t>
+          <t>Acht de minister het vooropgestelde budget voor de subsidie voldoende?</t>
         </is>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9544000029563904</v>
+        <v>0.9221016764640808</v>
       </c>
       <c r="D81" t="n">
-        <v>0.04559999704360962</v>
+        <v>0.07789832353591919</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Geldt de onverenigbaarheid tussen het mandaat van districtsraadslid en het mandaat van voorzitter of lid van het bijzonder comité voor de sociale dienst?</t>
+          <t>Acht de minister het vooropgestelde budget voor de subsidie voldoende?</t>
         </is>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9545018672943115</v>
+        <v>0.9221016764640808</v>
       </c>
       <c r="D82" t="n">
-        <v>0.04549813270568848</v>
+        <v>0.07789832353591919</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Kan een overzicht gegeven worden van de financiering van de aanpak van die knelpunten in de provincie Vlaams-Brabant?</t>
+          <t>Welk aandeel van deze gronden?</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9568672180175781</v>
+        <v>0.9245500564575195</v>
       </c>
       <c r="D83" t="n">
-        <v>0.04313278198242188</v>
+        <v>0.07544994354248047</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Werden alle mandaten van de bestuursraden die door middel van verkiezingen, georganiseerd in april van dit jaar, voor alle erediensten ingevuld?</t>
+          <t>Wanneer zal de volgende en zevende oproep plaatsvinden?</t>
         </is>
       </c>
       <c r="B84" t="n">
         <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>0.9596102833747864</v>
+        <v>0.9316099286079407</v>
       </c>
       <c r="D84" t="n">
-        <v>0.04038971662521362</v>
+        <v>0.06839007139205933</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Het Vlaams Vredesinstituut publiceerde in 2018 een rapport (‘Een schot in de roos?</t>
+          <t>Kan de minister een inschatting geven over de jaarlijkse meerkosten om alle vroegere rob-plaatsen voor zware zorgprofielen om te zetten naar rvt-plaatsen?</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9604334235191345</v>
+        <v>0.9333664774894714</v>
       </c>
       <c r="D85" t="n">
-        <v>0.03956657648086548</v>
+        <v>0.06663352251052856</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Indien dit niet het geval is, kan de minister een geüpdatet plan van aanpak met timing en budget geven?</t>
+          <t>Wat zijn de grootste hordes die nog genomen moeten worden om de deadline wel te halen?</t>
         </is>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9618756771087646</v>
+        <v>0.9350074529647827</v>
       </c>
       <c r="D86" t="n">
-        <v>0.03812432289123535</v>
+        <v>0.06499254703521729</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Wat zijn de gevolgen van de niet-naleving van de termijn van 30 dagen door de administratie?</t>
+          <t>Is het vooropstelde budget nog steeds haalbaar op basis van de al ingediende subsidieaanvragen?</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9618882536888123</v>
+        <v>0.9353166222572327</v>
       </c>
       <c r="D87" t="n">
-        <v>0.03811174631118774</v>
+        <v>0.06468337774276733</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Zijn er minderjarigen met een snel degeneratieve aandoening die geen PAB kregen omdat hun ziekte niet in aanmerking kwam?</t>
+          <t>Waarvoor wordt dit ‘overig aangegeven areaal’ ingezet? Graag per categorie van gebruik?</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9626314043998718</v>
+        <v>0.9356328248977661</v>
       </c>
       <c r="D88" t="n">
-        <v>0.03736859560012817</v>
+        <v>0.06436717510223389</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Geldt de onverenigbaarheid tussen het mandaat van districtsraadslid en het mandaat van provincieraadslid?</t>
+          <t>Is er nog een ruimere evaluatie gepland van de heraanleg van de Tiensepoort en tegen wanneer zal die evaluatie klaar zijn?</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9626580476760864</v>
+        <v>0.9359602928161621</v>
       </c>
       <c r="D89" t="n">
-        <v>0.03734195232391357</v>
+        <v>0.06403970718383789</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Wordt de beoogde ambitie van 150 toeleidingen per jaar gehaald?</t>
+          <t>b) Hoe kijkt de minister naar die cijfers?</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9631533026695251</v>
+        <v>0.9359674453735352</v>
       </c>
       <c r="D90" t="n">
-        <v>0.03684669733047485</v>
+        <v>0.06403255462646484</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>c) Wat voor type betreft de geplande warmtebron?</t>
+          <t>Het is voor VRT niet duidelijk wat precies bedoeld wordt met ‘hoeveel sportwedstrijden en -competities’ er werden uitgezonden.</t>
         </is>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9637096524238586</v>
+        <v>0.9367933869361877</v>
       </c>
       <c r="D91" t="n">
-        <v>0.03629034757614136</v>
+        <v>0.06320661306381226</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Welk engagement wordt van de betrokken gemeenten verwacht bij het wegwerken besturen, of een engagement om lokale infrastructuur aanliggend aan het schoolrouteknelpunt op een gewestweg tegelijk mee aan te pakken?</t>
+          <t>Voor de telewerkmiddelen is het niet mogelijk om na te gaan hoeveel personeelsleden daarvan gebruik hebben gemaakt.</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9648166298866272</v>
+        <v>0.9434449672698975</v>
       </c>
       <c r="D92" t="n">
-        <v>0.0351833701133728</v>
+        <v>0.05655503273010254</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Kan de minister garanderen dat die evaluatie zeker nog dit jaar wordt afgerond en er deze legislatuur nog de nodige aanpassingen gedaan worden?</t>
+          <t>Is er een definitie beschikbaar van ‘onvoldoende aangepaste ondersteuning’?</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9657052159309387</v>
+        <v>0.9437419772148132</v>
       </c>
       <c r="D93" t="n">
-        <v>0.03429478406906128</v>
+        <v>0.05625802278518677</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Moet de stemming over de toegestane maximumprijs plaatshebben in de openbare of in de besloten vergadering?</t>
+          <t>c) Tegen wanneer wordt een nieuwe versie gepland?</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9668937921524048</v>
+        <v>0.9450353384017944</v>
       </c>
       <c r="D94" t="n">
-        <v>0.03310620784759521</v>
+        <v>0.05496466159820557</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>b) Kan de minister ook een verder plan van aanpak met timing en budget geven?</t>
+          <t>Wat de vangplanken betreft die geplaatst werden voor 1 januari 2020:a) Wanneer werden die al bestaande beschermplanken nog eens gecontroleerd en onderhouden?</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.96720290184021</v>
+        <v>0.9467188715934753</v>
       </c>
       <c r="D95" t="n">
-        <v>0.03279709815979004</v>
+        <v>0.05328112840652466</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>(zie voor aandeel onderwijs: SD2)SD5 We versterken de aandacht voor taalstimulering en vroeggeletterdheid bij wie professioneel bezig is met baby’s, peuters en kleuters en stimuleren interactief voorlezen.</t>
+          <t>a) Een overzicht van het aantal LDE-ondernemingen, opgedeeld naar hoeveel LDE’ers er actief zijn binnen de onderneming (ondernemingen met minder dan 5, 5-10, 11-20, 21-50, 51-100, 100+).</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9677677750587463</v>
+        <v>0.9474017024040222</v>
       </c>
       <c r="D96" t="n">
-        <v>0.03223222494125366</v>
+        <v>0.05259829759597778</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>(zie voor aandeel onderwijs: SD2)SD5 We versterken de aandacht voor taalstimulering en vroeggeletterdheid bij wie professioneel bezig is met baby’s, peuters en kleuters en stimuleren interactief voorlezen.</t>
+          <t>Is er al een concrete datum meegedeeld?</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.9677677750587463</v>
+        <v>0.9474270343780518</v>
       </c>
       <c r="D97" t="n">
-        <v>0.03223222494125366</v>
+        <v>0.05257296562194824</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Het niet beschikbaar zijn van een proper toilet met de nodige voorzieningen kan voor mensen met bepaalde aandoeningen en bij wie er soms plots een dringende nood is, zelfs ronduit problematisch zijn.</t>
+          <t>Welke timing is er vooropgesteld om de consolidatieoefening, het hervormingsvoorstel en het uitvoeringsplan rond te hebben?</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9678625464439392</v>
+        <v>0.9486436247825623</v>
       </c>
       <c r="D98" t="n">
-        <v>0.03213745355606079</v>
+        <v>0.05135637521743774</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Ging het vooral over mensen die in de slachthuizen werken of waren het eerder mensen die niet in het slachthuis werkten, maar de dieren vervoerden of door eigenaars van de dieren?</t>
+          <t>Wat is de evolutie sinds 2021?</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99" t="n">
-        <v>0.968762993812561</v>
+        <v>0.9487893581390381</v>
       </c>
       <c r="D99" t="n">
-        <v>0.03123700618743896</v>
+        <v>0.05121064186096191</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Wat kan worden afgeleid uit de data die momenteel worden verzameld door de diverse telpalen?</t>
+          <t>Zijn er naast deze 14,2 miljoen euro nog andere subsidies of financiële ondersteuning gegeven aan Sappi?</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9692338109016418</v>
+        <v>0.9504262804985046</v>
       </c>
       <c r="D100" t="n">
-        <v>0.03076618909835815</v>
+        <v>0.04957371950149536</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Als er sleutelcompetenties al van in het basisonderwijs en ook in bepaalde graden in het secundair onderwijs worden leeggelaten, in hoeverre heeft het dan zin dat we aan (het geheel van) die zestien sleutelcompetenties vasthouden?</t>
+          <t>Welke budgetten werden al besteed en welke dienen nog gereserveerd te worden voor de knelpunten die nog uitgevoerd dienen te worden?</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9710237383842468</v>
+        <v>0.9522846937179565</v>
       </c>
       <c r="D101" t="n">
-        <v>0.02897626161575317</v>
+        <v>0.04771530628204346</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>- Wat is de (huidige) omvang van de markt voor tweedehandsmobiliteitshulpmiddelen?</t>
+          <t>Wanneer is de minister hiervoor in overleg gegaan met zijn federale collega-minister?</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>0.9719222187995911</v>
+        <v>0.9527001976966858</v>
       </c>
       <c r="D102" t="n">
-        <v>0.02807778120040894</v>
+        <v>0.04729980230331421</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Zou het zinvol zijn om een algemeen beleidskader uit te werken voor alle zorginstellingen?</t>
+          <t>Wordt die voorraad nog verder aangevuld tegen de winter of is dat de capaciteit om voorbereid te zijn?</t>
         </is>
       </c>
       <c r="B103" t="n">
         <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>0.972353458404541</v>
+        <v>0.9527662992477417</v>
       </c>
       <c r="D103" t="n">
-        <v>0.02764654159545898</v>
+        <v>0.0472337007522583</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Zijn er meerdere kandidaten van wie het dossiers volledig en ontvankelijk zijn, dan worden de dossiers getoetst aan inhoudelijke criteria en kent de VRM de licentie toe binnen de 120 dagen na publicatie van de oproep tot kandidaatstelling.</t>
+          <t>Kan de minister al een indicatieve timing geven voor het verhogen en vervangen van de bruggen?</t>
         </is>
       </c>
       <c r="B104" t="n">
         <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>0.9726055264472961</v>
+        <v>0.953096330165863</v>
       </c>
       <c r="D104" t="n">
-        <v>0.02739447355270386</v>
+        <v>0.04690366983413696</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Heeft de minister ook een ondersteunend kader vooropgesteld voor de scholen?</t>
+          <t>Wat is de intensiteit op het drukste uur langs de Lierselei?</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" t="n">
-        <v>0.972666323184967</v>
+        <v>0.9535861611366272</v>
       </c>
       <c r="D105" t="n">
-        <v>0.02733367681503296</v>
+        <v>0.0464138388633728</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Heeft de minister ook een ondersteunend kader vooropgesteld voor de scholen?</t>
+          <t>c) Is de langere wachttijd voor een oproep merkbaar bij het aantal aanvragen?</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>0.972666323184967</v>
+        <v>0.9537416696548462</v>
       </c>
       <c r="D106" t="n">
-        <v>0.02733367681503296</v>
+        <v>0.04625833034515381</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Zijn de diensten van de minister in het bezit van een globaal overzicht van alle geopende asielcentra sinds 2019? Zo ja, kan de minister die lijst toevoegen bij zijn antwoord?</t>
+          <t>Wanneer zullen die werken plaatsvinden?</t>
         </is>
       </c>
       <c r="B107" t="n">
         <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>0.9727662801742554</v>
+        <v>0.956331193447113</v>
       </c>
       <c r="D107" t="n">
-        <v>0.02723371982574463</v>
+        <v>0.04366880655288696</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Wanneer mogen wij eindelijk dat actieplan tegen schooluitval, zoals vermeld in het regeerakkoord, verwachten?</t>
+          <t>Wanneer werden de metingen precies uitgevoerd?</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108" t="n">
-        <v>0.9731479287147522</v>
+        <v>0.9566543102264404</v>
       </c>
       <c r="D108" t="n">
-        <v>0.0268520712852478</v>
+        <v>0.04334568977355957</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Kan er eventueel een overzicht gegeven worden van het aantal deelnemers per knelpuntberoep, per gender en leeftijdscategorie?</t>
+          <t>Hoe groot is het ‘kort’ ziekteverzuim bij De Lijn?</t>
         </is>
       </c>
       <c r="B109" t="n">
         <v>1</v>
       </c>
       <c r="C109" t="n">
-        <v>0.973509669303894</v>
+        <v>0.9583697915077209</v>
       </c>
       <c r="D109" t="n">
-        <v>0.02649033069610596</v>
+        <v>0.04163020849227905</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Is alles aangewend zoals de minister begroot had of is er onderbenutting?</t>
+          <t>Wat zijn de criteria om een werkzoekende een ticket individueel maatwerk voor 2 jaar te geven in plaats van een ticket voor individueel maatwerk voor een traject van 5 jaar?</t>
         </is>
       </c>
       <c r="B110" t="n">
         <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>0.9736652374267578</v>
+        <v>0.9583955407142639</v>
       </c>
       <c r="D110" t="n">
-        <v>0.02633476257324219</v>
+        <v>0.04160445928573608</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Beschikt de minister over de effectieve waarde (in euro) van een opcentiem voor elke gemeente?</t>
+          <t>Wanneer zal er in een definitieve afsluiting worden voorzien?</t>
         </is>
       </c>
       <c r="B111" t="n">
         <v>1</v>
       </c>
       <c r="C111" t="n">
-        <v>0.9737228751182556</v>
+        <v>0.9591220617294312</v>
       </c>
       <c r="D111" t="n">
-        <v>0.02627712488174438</v>
+        <v>0.04087793827056885</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Kan de minister een actuele evaluatie geven van het IBM ‘SMAS’-platform dat grijze punten detecteert in het wegennetwerk?</t>
+          <t>Welke budgetten werden uitgetrokken om de toepassing te bouwen en uit te rollen?</t>
         </is>
       </c>
       <c r="B112" t="n">
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>0.9739218354225159</v>
+        <v>0.9594151377677917</v>
       </c>
       <c r="D112" t="n">
-        <v>0.02607816457748413</v>
+        <v>0.04058486223220825</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>a) Tegen wanneer zal de minister die oefening klaar hebben?</t>
+          <t>Kan de minister een overzicht geven van de ontvangen klachten voor mei, augustus en september 2023?</t>
         </is>
       </c>
       <c r="B113" t="n">
         <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>0.9743820428848267</v>
+        <v>0.9597422480583191</v>
       </c>
       <c r="D113" t="n">
-        <v>0.02561795711517334</v>
+        <v>0.04025775194168091</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Kan de minister een update van de lijst bezorgen van het aantal ongevallen op de gevaarlijke punten in West-Vlaanderen voor 2019, 2020, 2021, 2022 en 2023?</t>
+          <t>Is er een evaluatie gebeurd over de berekening van de beloningen?</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>0.9744972586631775</v>
+        <v>0.9631454944610596</v>
       </c>
       <c r="D114" t="n">
-        <v>0.02550274133682251</v>
+        <v>0.03685450553894043</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>a) Op basis waarvan is de lijst van producten waarvoor men een vergoeding kan krijgen, opgesteld?</t>
+          <t>Werden alle beschikbare leerwerkplekken ingevuld?</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" t="n">
-        <v>0.97453373670578</v>
+        <v>0.9645271897315979</v>
       </c>
       <c r="D115" t="n">
-        <v>0.02546626329421997</v>
+        <v>0.0354728102684021</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>882 van 6 september 2023 verwijst minister Weyts mij door naar het Agentschap Integratie en Inburgering voor de volgende vraag: “Met een CNaVT-certificaat kan een vrijstelling verkregen worden bij het Vlaamse inburgeringsprogramma voor het luik kennis van het Nederlands voor inburgeraars.” Hoe vaak werd in de voorbije 5 jaar een vrijstelling voor het luik Nederlands verleend op basis van dit CNaVT-certificaat?</t>
+          <t>Werden alle beschikbare leerwerkplekken ingevuld?</t>
         </is>
       </c>
       <c r="B116" t="n">
         <v>1</v>
       </c>
       <c r="C116" t="n">
-        <v>0.974638819694519</v>
+        <v>0.9645271897315979</v>
       </c>
       <c r="D116" t="n">
-        <v>0.02536118030548096</v>
+        <v>0.0354728102684021</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Hoe vaak werd de Toegankelijkheidswijzer sinds de lancering geraadpleegd?</t>
+          <t>Wanneer kunnen we de analyse in het parlement verwachten?</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>0.9746556878089905</v>
+        <v>0.9686517119407654</v>
       </c>
       <c r="D117" t="n">
-        <v>0.02534431219100952</v>
+        <v>0.03134828805923462</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>e) Wanneer zal dat op de raad van bestuur komen?</t>
+          <t>a) Kan de minister een lijst geven - ingedeeld naar provincie en naar gemeente of stad - van alle kruispunten die in hun totaliteit (dus alle takken) volledig conflictvrij zijn (in absolute aantallen en procentueel)?</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>0.9747529625892639</v>
+        <v>0.969679057598114</v>
       </c>
       <c r="D118" t="n">
-        <v>0.02524703741073608</v>
+        <v>0.03032094240188599</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>a) Kan de minister een overzicht geven per jaar in de periode 2019-2023?</t>
+          <t>Welke vertragingen zijn er gemiddeld?</t>
         </is>
       </c>
       <c r="B119" t="n">
         <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>0.974821925163269</v>
+        <v>0.9712814092636108</v>
       </c>
       <c r="D119" t="n">
-        <v>0.02517807483673096</v>
+        <v>0.02871859073638916</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Kan een jaarlijks overzicht gegeven worden voor deze legislatuur van welke projecten uitgevoerd konden worden en welke financiering daarvoor vooropgesteld werd?</t>
+          <t>Hoe groot is het ‘middellang’ ziekteverzuim bij De Lijn?</t>
         </is>
       </c>
       <c r="B120" t="n">
         <v>1</v>
       </c>
       <c r="C120" t="n">
-        <v>0.9748835563659668</v>
+        <v>0.9722506999969482</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0251164436340332</v>
+        <v>0.02774930000305176</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Kan de minister per jaar en per provincie een onderverdeling maken voor de periode 2018 tot heden met enerzijds nieuwe aanmeldingen bij Dyzo en anderzijds lopende dossiers waarbij een beroep werd gedaan op Dyzo, maar de aanmelding al plaatsvond in het verleden? Zo ja, zijn de effecten van de COVID-19-crisis op deze manier duidelijk zichtbaar? Zo ja, zijn de effecten van de loonindexering, de stijgende grondstof- en bouwkosten en de energiecrisis zichtbaar in de cijfers?</t>
+          <t>Hoe staat de minister tegenover een snelheidsverlaging naar 50 km/u op de Lierselei, en meer in het algemeen op wegen waar 70 km/u de maximumsnelheid is en er geen vrijliggend fietspad aanwezig is?</t>
         </is>
       </c>
       <c r="B121" t="n">
         <v>0</v>
       </c>
       <c r="C121" t="n">
-        <v>0.9754484295845032</v>
+        <v>0.9733081459999084</v>
       </c>
       <c r="D121" t="n">
-        <v>0.02455157041549683</v>
+        <v>0.02669185400009155</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Werd de ambitie om in elke gemeente, waar mogelijk, nodig en nuttig, in ten minste één speelzone te voorzien, ondertussen behaald?</t>
+          <t>Wat was de verwachte duur van de verwijdering?</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122" t="n">
-        <v>0.9757347106933594</v>
+        <v>0.973653256893158</v>
       </c>
       <c r="D122" t="n">
-        <v>0.02426528930664062</v>
+        <v>0.02634674310684204</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>a) Zijn er provincies met opvallend veel dan wel opvallend weinig speelzones?</t>
+          <t>Wat zal de (na) bestemming zijn van de strook verharding?</t>
         </is>
       </c>
       <c r="B123" t="n">
         <v>0</v>
       </c>
       <c r="C123" t="n">
-        <v>0.976212739944458</v>
+        <v>0.9762275218963623</v>
       </c>
       <c r="D123" t="n">
-        <v>0.02378726005554199</v>
+        <v>0.0237724781036377</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Hoe lang duurde het telkens om de reparatie te voltooien en wat was de gemiddelde ‘buiten dienst’-tijd?</t>
+          <t>Kan de minister een overzicht geven van de resultaten van de zesde oproep voor huursubsidies in het onderwijs?</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>0.9771578311920166</v>
+        <v>0.9772765636444092</v>
       </c>
       <c r="D124" t="n">
-        <v>0.0228421688079834</v>
+        <v>0.02272343635559082</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Uitbreiding huursysteem thuiszorg- Welke andere leeftijdsgroepen komen potentieel in aanmerking voor opname in het huidige huursysteem?</t>
+          <t>Wat is de vooropgestelde datum van de effectieve inwerkingtreding?</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" t="n">
-        <v>0.9777116775512695</v>
+        <v>0.977390468120575</v>
       </c>
       <c r="D125" t="n">
-        <v>0.02228832244873047</v>
+        <v>0.02260953187942505</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Kan de minister een overzicht geven per jaar in de periode 2019-2023?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem dat op dit knelpunt gesignaleerd was, welke maatregelen hier genomen werden, welke resultaten dit oplevert en hoeveel het budget bedroeg?</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>0.9777145385742188</v>
+        <v>0.9775400161743164</v>
       </c>
       <c r="D126" t="n">
-        <v>0.02228546142578125</v>
+        <v>0.02245998382568359</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>d) Is er ook een opmerkelijk verschil van gerapporteerde overtredingen vast te stellen in slachthuizen waar nog geen Vlaamse DMO’s actief zijn ten aanzien van zij die wel toezicht hebben van Vlaamse DMO’s?</t>
+          <t>De federale overheid bleef na de zesde staatshervorming instaan voor de financiering Om hoeveel woongelegenheden gaat dit in Vlaanderen?</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C127" t="n">
-        <v>0.9777758717536926</v>
+        <v>0.9776579141616821</v>
       </c>
       <c r="D127" t="n">
-        <v>0.02222412824630737</v>
+        <v>0.02234208583831787</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Wat was het resultaat van de evaluatie?</t>
+          <t>Wanneer zal de vergunning van de tramstelplaats in de Jan Van de Wouwerstraat in Hoboken verlopen?</t>
         </is>
       </c>
       <c r="B128" t="n">
         <v>0</v>
       </c>
       <c r="C128" t="n">
-        <v>0.9777873754501343</v>
+        <v>0.9778242707252502</v>
       </c>
       <c r="D128" t="n">
-        <v>0.02221262454986572</v>
+        <v>0.02217572927474976</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Worden op die manier die leeg gelaten sleutelcompetenties dan niet gereduceerd tot restjescompetenties?</t>
+          <t>Hoe groot is het ‘globaal’ ziekteverzuim bij De Lijn?</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>0.97852623462677</v>
+        <v>0.9784333109855652</v>
       </c>
       <c r="D129" t="n">
-        <v>0.02147376537322998</v>
+        <v>0.02156668901443481</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Zal dat ook werken aan specifiek evidence informed materiaal over en voor de B-stroom?</t>
+          <t>Is er een termijn bepaald van hoelang de persoon met een handicap ondersteund moet worden door bijvoorbeeld een woonzorgcentrum of een psychiatrische instelling?</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C130" t="n">
-        <v>0.9785619974136353</v>
+        <v>0.9790761470794678</v>
       </c>
       <c r="D130" t="n">
-        <v>0.02143800258636475</v>
+        <v>0.02092385292053223</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Kan de minister een geanonimiseerde lijst bezorgen van de ingediende steunaanvragen voor de uitkoopregeling varkens per provincie, met per bedrijf vermelding van het aantal dieren, het huidige type of de leeftijd van de stal?</t>
+          <t>Klopt het dat de files voor het gemotoriseerd verkeer op de Tiensesteenweg langer zijn geworden ten gevolge van de heraanleg van de Tiensepoort?</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" t="n">
-        <v>0.9788387417793274</v>
+        <v>0.9797599911689758</v>
       </c>
       <c r="D131" t="n">
-        <v>0.02116125822067261</v>
+        <v>0.02024000883102417</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Werden er berekeningen gemaakt van de effecten op de snelwegen die aansluiten op de R0 en dus op de dagdagelijkse pendelaar?</t>
+          <t>Zijn de files richting Tiensepoort op de vesten verminderd, vergroot of hetzelfde gebleven?</t>
         </is>
       </c>
       <c r="B132" t="n">
         <v>0</v>
       </c>
       <c r="C132" t="n">
-        <v>0.9791314601898193</v>
+        <v>0.9817548394203186</v>
       </c>
       <c r="D132" t="n">
-        <v>0.02086853981018066</v>
+        <v>0.0182451605796814</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>b) Kan de minister ook een verdere aanpak, timing en budget geven?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem van dit knelpunt, welke maatregelen hier genomen worden, welke verdere stappen en timing hierin worden vooropgesteld en hoeveel het budget bedraagt?</t>
         </is>
       </c>
       <c r="B133" t="n">
         <v>0</v>
       </c>
       <c r="C133" t="n">
-        <v>0.9792225360870361</v>
+        <v>0.9820739030838013</v>
       </c>
       <c r="D133" t="n">
-        <v>0.02077746391296387</v>
+        <v>0.01792609691619873</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>- Hoe kan de vergoedbaarheid van tweedehandshulpmiddelen opgenomen worden in het bestaande derdebetalerssysteem?</t>
+          <t>Als de 100 miljoen niet gebruikt wordt, wat zal de minister dan met het overschot van dat budget doen?</t>
         </is>
       </c>
       <c r="B134" t="n">
         <v>0</v>
       </c>
       <c r="C134" t="n">
-        <v>0.9792382121086121</v>
+        <v>0.9824368953704834</v>
       </c>
       <c r="D134" t="n">
-        <v>0.02076178789138794</v>
+        <v>0.0175631046295166</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Wat is de reden dat de lift opnieuw buiten dienst is?</t>
+          <t>Wat zijn per grond nog de geplande initiatieven?</t>
         </is>
       </c>
       <c r="B135" t="n">
         <v>0</v>
       </c>
       <c r="C135" t="n">
-        <v>0.9805760979652405</v>
+        <v>0.9827114939689636</v>
       </c>
       <c r="D135" t="n">
-        <v>0.01942390203475952</v>
+        <v>0.01728850603103638</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Beschikt de minister over cijfers over het aantal ondernemingen in moeilijkheden die begeleid werden door Dyzo in 2023? Zo ja, kan de minister per provincie de beschikbare cijfers vergelijken met eenzelfde periode van 2019 tot 2023?</t>
+          <t>Zijn er al resultaten beschikbaar die gedeeld kunnen worden?</t>
         </is>
       </c>
       <c r="B136" t="n">
         <v>1</v>
       </c>
       <c r="C136" t="n">
-        <v>0.9805780649185181</v>
+        <v>0.9833329916000366</v>
       </c>
       <c r="D136" t="n">
-        <v>0.01942193508148193</v>
+        <v>0.01666700839996338</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Welke timing wordt vooropgesteld om alle mogelijke knelpunten weg te werken?</t>
+          <t>b) Welke plaatsen werden gerealiseerd tussen 1 januari 2020 en heden?</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" t="n">
-        <v>0.9810552597045898</v>
+        <v>0.9837765097618103</v>
       </c>
       <c r="D137" t="n">
-        <v>0.01894474029541016</v>
+        <v>0.0162234902381897</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Wat is de inschatting van de Dienst Controle Strategische Goederen om de vergunning goed te keuren?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem stappen en timing hierin worden vooropgesteld?</t>
         </is>
       </c>
       <c r="B138" t="n">
         <v>0</v>
       </c>
       <c r="C138" t="n">
-        <v>0.9812493920326233</v>
+        <v>0.9839385151863098</v>
       </c>
       <c r="D138" t="n">
-        <v>0.01875060796737671</v>
+        <v>0.01606148481369019</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Wat is de inschatting van de Dienst Controle Strategische Goederen om de vergunning goed te keuren?</t>
+          <t>In verband met de kostprijs en besparing daarop:a) Wat was de jaarlijkse investeringskostprijs in de voorbije 5 jaar om meer gericht te kunnen strooien?</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>0.9812493920326233</v>
+        <v>0.9839608669281006</v>
       </c>
       <c r="D139" t="n">
-        <v>0.01875060796737671</v>
+        <v>0.01603913307189941</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Wat is de inschatting van de Dienst Controle Strategische Goederen om de vergunning goed te keuren?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met SUV’s en het aantal ingeschreven SUV’s?</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C140" t="n">
-        <v>0.9812493920326233</v>
+        <v>0.9844368696212769</v>
       </c>
       <c r="D140" t="n">
-        <v>0.01875060796737671</v>
+        <v>0.01556313037872314</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Wat is de inschatting van de Dienst Controle Strategische Goederen om de vergunning goed te keuren?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met SUV’s en het aantal ingeschreven SUV’s?</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C141" t="n">
-        <v>0.9812493920326233</v>
+        <v>0.9844368696212769</v>
       </c>
       <c r="D141" t="n">
-        <v>0.01875060796737671</v>
+        <v>0.01556313037872314</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Wat zijn de resultaten van het zachte handhavingstraject dat werd gelopen?</t>
+          <t>Waren er in het schooljaar 2022-2023 tekorten aan leerwerkplekken?</t>
         </is>
       </c>
       <c r="B142" t="n">
         <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>0.9819642305374146</v>
+        <v>0.9846816062927246</v>
       </c>
       <c r="D142" t="n">
-        <v>0.01803576946258545</v>
+        <v>0.01531839370727539</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>- Wat is de gemiddelde gebruiksduur van mobiliteitshulpmiddelen voor deze leeftijdsgroepen?</t>
+          <t>Vroeger werd er ‘wild’ gestrooid maar de laatste jaren meer gericht op basis van weersvoorspellingen, metingen en met materiaal dat beter bepaalt hoeveel en waar exact er gestrooid moet worden.</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C143" t="n">
-        <v>0.9820942282676697</v>
+        <v>0.984683096408844</v>
       </c>
       <c r="D143" t="n">
-        <v>0.01790577173233032</v>
+        <v>0.01531690359115601</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>a) Wat is de huidige situatie met betrekking tot de omgevingsvergunning voor deze werken?</t>
+          <t>a) Een overzicht van het aantal maatwerkondernemingen, opgedeeld naar hoeveel maatwerkers er actief zijn binnen de onderneming.</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C144" t="n">
-        <v>0.9822083115577698</v>
+        <v>0.9848832488059998</v>
       </c>
       <c r="D144" t="n">
-        <v>0.01779168844223022</v>
+        <v>0.01511675119400024</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Zijn er procentueel meer inschrijvingen dan het voorgaande jaar (schooljaar 2022-2023) omdat we twijfelaars mee aan boord trekken?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem van dit knelpunt, welke maatregelen hier genomen zullen worden, welke verdere stappen en timing hierin worden vooropgesteld en hoeveel het budget bedraagt?</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145" t="n">
-        <v>0.9824322462081909</v>
+        <v>0.9850908517837524</v>
       </c>
       <c r="D145" t="n">
-        <v>0.01756775379180908</v>
+        <v>0.01490914821624756</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Werden nog bijkomende budgetten uitgetrokken voor een verdere uitrol?</t>
+          <t>Welke woonzorgvoorzieningen kregen een Kappa-controle in de jaren 2021, 2022 en tot op heden in 2023?</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146" t="n">
-        <v>0.982529878616333</v>
+        <v>0.9851527214050293</v>
       </c>
       <c r="D146" t="n">
-        <v>0.01747012138366699</v>
+        <v>0.0148472785949707</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Kan de minister, eveneens opgesplitst per kabinet, het totaalaantal kabinetsmedewerkers dat opnieuw vertrok opsommen?</t>
+          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem van dit knelpunt, welk onderzoek hier concreet loopt, welke verdere stappen en timing hierin worden vooropgesteld en hoeveel het budget bedraagt?</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147" t="n">
-        <v>0.9829628467559814</v>
+        <v>0.9854530692100525</v>
       </c>
       <c r="D147" t="n">
-        <v>0.01703715324401855</v>
+        <v>0.01454693078994751</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Dit budgettair uitsplitsen is bijgevolg niet mogelijk.” Welk budget werd er voor 2023 gereserveerd voor de bestrijding van al deze invasieve exoten waarvan er overigens - denk bijvoorbeeld alleen al maar aan de Aziatische hoornaar - steeds meer opduiken?</t>
+          <t>VDAB heeft geen data over het aantal “oudkomers” die in de voorbije 10 jaar verplicht werden door VDAB om een inburgeringstraject te volgen, wel hoeveel keer werkzoekenden de opdracht kregen door de VDAB bemiddelaar om een inburgeringstraject te volgen sinds de hernieuwde samenwerking in 2022.</t>
         </is>
       </c>
       <c r="B148" t="n">
         <v>1</v>
       </c>
       <c r="C148" t="n">
-        <v>0.9830681681632996</v>
+        <v>0.9855421781539917</v>
       </c>
       <c r="D148" t="n">
-        <v>0.01693183183670044</v>
+        <v>0.0144578218460083</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Maar op het niveau van het kleuteronderwijs zijn er toch geen peilingen of Vlaamse centrale toetsen?’5.</t>
+          <t>b) Wat was de besparing in de hoeveelheid strooizout, kostprijs van strooizout en ook werkuren door dat meer gericht strooien?</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C149" t="n">
-        <v>0.9831470847129822</v>
+        <v>0.985586404800415</v>
       </c>
       <c r="D149" t="n">
-        <v>0.01685291528701782</v>
+        <v>0.01441359519958496</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Werd er al een model-IDO aangepast door het VAPH? Zo ja, om welk type model-IDO gaat het en wat werd er aangepast?</t>
+          <t>Beschikt de minister over cijfers van het aantal aannemers dat zijn lidmaatschap stop wenst te zetten? Zo ja, kan hij die meedelen?</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C150" t="n">
-        <v>0.9831493496894836</v>
+        <v>0.9857012033462524</v>
       </c>
       <c r="D150" t="n">
-        <v>0.01685065031051636</v>
+        <v>0.01429879665374756</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Wanneer wordt de nieuwe regeling opengesteld en wat zal de indieningsdeadline zijn?</t>
+          <t>Wanneer zal De Lijn de alternatieve stelplaatsstudie opleveren?</t>
         </is>
       </c>
       <c r="B151" t="n">
         <v>0</v>
       </c>
       <c r="C151" t="n">
-        <v>0.9833998084068298</v>
+        <v>0.9858801960945129</v>
       </c>
       <c r="D151" t="n">
-        <v>0.01660019159317017</v>
+        <v>0.01411980390548706</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Wat is nu eigenlijk de concrete stand van zaken wat betreft deze beheerregeling?</t>
+          <t>Wanneer verwacht de minister het resultaat van deze studie?</t>
         </is>
       </c>
       <c r="B152" t="n">
         <v>0</v>
       </c>
       <c r="C152" t="n">
-        <v>0.9834437370300293</v>
+        <v>0.9860509037971497</v>
       </c>
       <c r="D152" t="n">
-        <v>0.0165562629699707</v>
+        <v>0.01394909620285034</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>b) Klopt het dat de federale DMO’s opmerkelijk minder overtredingen rapporteren op ogenblikken dat de Vlaamse DMO’s niet aanwezig zijn?</t>
+          <t>Wanneer kunnen de richtlijnen daaromtrent verwacht worden?</t>
         </is>
       </c>
       <c r="B153" t="n">
         <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>0.9836789965629578</v>
+        <v>0.9861765503883362</v>
       </c>
       <c r="D153" t="n">
-        <v>0.01632100343704224</v>
+        <v>0.01382344961166382</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>a) Verwacht de minister een stijgend aantal bedrijven in moeilijkheden door deze crisissen?</t>
+          <t>Is de minister tevreden met de geografische spreiding van de aanvragen?</t>
         </is>
       </c>
       <c r="B154" t="n">
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>0.9837820529937744</v>
+        <v>0.9866304993629456</v>
       </c>
       <c r="D154" t="n">
-        <v>0.01621794700622559</v>
+        <v>0.01336950063705444</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Als er onderbenutting is van de gereserveerde middelen, hoe zal de minister dat aanwenden?</t>
+          <t>Waarvoor is het bedrag van 9 miljoen euro exact bestemd?</t>
         </is>
       </c>
       <c r="B155" t="n">
         <v>0</v>
       </c>
       <c r="C155" t="n">
-        <v>0.9838299155235291</v>
+        <v>0.9868029952049255</v>
       </c>
       <c r="D155" t="n">
-        <v>0.01617008447647095</v>
+        <v>0.01319700479507446</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Kan een update worden gegeven van bruggen in beheer van het AWV, DVW (De Vlaamse Waterweg), MOW, … per provincie waar een fietssnelweg over loopt?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal 6- tot 18-jarige inwoners in de provincie?</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C156" t="n">
-        <v>0.9839698672294617</v>
+        <v>0.987443745136261</v>
       </c>
       <c r="D156" t="n">
-        <v>0.01603013277053833</v>
+        <v>0.01255625486373901</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Welke onderzoeksresultaten heeft het everzwijnproefproject in Genk tot op heden opgeleverd, hoe zullen ze beleidsmatig vertaald worden, en hoeveel bedraagt de kostprijs van het proefproject?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal 6- tot 18-jarige inwoners in de provincie?</t>
         </is>
       </c>
       <c r="B157" t="n">
         <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>0.9840667247772217</v>
+        <v>0.987443745136261</v>
       </c>
       <c r="D157" t="n">
-        <v>0.01593327522277832</v>
+        <v>0.01255625486373901</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie, het probleem stappen en timing worden vooropgesteld?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal 6- tot 18-jarige inwoners in de provincie?</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C158" t="n">
-        <v>0.9841694831848145</v>
+        <v>0.987443745136261</v>
       </c>
       <c r="D158" t="n">
-        <v>0.01583051681518555</v>
+        <v>0.01255625486373901</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Kan hij een overzicht geven van de budgettaire kostprijs daarvan?</t>
+          <t>Hoe verhoudt dat zich tot het totaalaantal bewoners in een woonzorgcentrum?</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C159" t="n">
-        <v>0.9841869473457336</v>
+        <v>0.9883245229721069</v>
       </c>
       <c r="D159" t="n">
-        <v>0.01581305265426636</v>
+        <v>0.01167547702789307</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Wat verwachten we van dat soort jongeren?</t>
+          <t>Welk subsidiebudget werd vrijgemaakt voor deze oproep?</t>
         </is>
       </c>
       <c r="B160" t="n">
         <v>0</v>
       </c>
       <c r="C160" t="n">
-        <v>0.9842554926872253</v>
+        <v>0.9884892106056213</v>
       </c>
       <c r="D160" t="n">
-        <v>0.01574450731277466</v>
+        <v>0.01151078939437866</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Als er een vertraging zit op de uitvoering, kan de minister dan een plan van aanpak en geüpdatete timing geven?</t>
+          <t>Wat is de laatste stand van zaken in de uitvoering van het akkoord dat door beide landen met bemiddeling van de EU gesloten werd?</t>
         </is>
       </c>
       <c r="B161" t="n">
         <v>0</v>
       </c>
       <c r="C161" t="n">
-        <v>0.9843016862869263</v>
+        <v>0.9889751672744751</v>
       </c>
       <c r="D161" t="n">
-        <v>0.01569831371307373</v>
+        <v>0.0110248327255249</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Kan een update gegeven worden over de 874 onveilige plekken op schoolroutes die gedetecteerd werden?</t>
+          <t>Hoe groot is het ‘lang’ ziekteverzuim bij De Lijn?</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C162" t="n">
-        <v>0.9847348928451538</v>
+        <v>0.9889914989471436</v>
       </c>
       <c r="D162" t="n">
-        <v>0.01526510715484619</v>
+        <v>0.01100850105285645</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>In welke budgetten dient nog te worden voorzien voor de knelpunten die nog moeten worden aangepakt?</t>
+          <t>Wat zijn de gevolgen gekoppeld aan het niet voldoen?</t>
         </is>
       </c>
       <c r="B163" t="n">
         <v>0</v>
       </c>
       <c r="C163" t="n">
-        <v>0.984847366809845</v>
+        <v>0.9895373582839966</v>
       </c>
       <c r="D163" t="n">
-        <v>0.01515263319015503</v>
+        <v>0.01046264171600342</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>In welke Vlaamse gemeenten zal het project verder uitgerold worden, op hoeveel euro wordt die uitrol voorlopig geraamd, welke cijfermatige doelstellingen worden vooropgesteld, wanneer is een eerste evaluatie van deze verdere uitrol gepland, en welke extra mensen zullen daarvoor door welke diensten aangeworven worden?</t>
+          <t>Wat zijn de gevolgen gekoppeld aan het niet voldoen?</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C164" t="n">
-        <v>0.984980583190918</v>
+        <v>0.9895373582839966</v>
       </c>
       <c r="D164" t="n">
-        <v>0.01501941680908203</v>
+        <v>0.01046264171600342</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Acht de minister dat bedrag voldoende of wordt in de toekomst in verdere financiële middelen voorzien?</t>
+          <t>Welke timing heeft de minister voor ogen om de actie in haar geheel af te ronden?</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C165" t="n">
-        <v>0.9849886894226074</v>
+        <v>0.989790141582489</v>
       </c>
       <c r="D165" t="n">
-        <v>0.01501131057739258</v>
+        <v>0.01020985841751099</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Is er ook fysieke bewaking door politionele ordediensten voor het Errerahuis (militaire politie…)?</t>
+          <t>En wie op basis van zijn functie een laptop, GSM of draagtas nodig heeft die krijgt er één.</t>
         </is>
       </c>
       <c r="B166" t="n">
         <v>0</v>
       </c>
       <c r="C166" t="n">
-        <v>0.9850356578826904</v>
+        <v>0.9897997379302979</v>
       </c>
       <c r="D166" t="n">
-        <v>0.01496434211730957</v>
+        <v>0.01020026206970215</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Kan de minister bevestigen dat bovenvermelde Zoutleeuwse deelgemeenten enkel door functionele lijnen bediend worden?</t>
+          <t>Over welke grond (locatie, hoeveelheid, vervuilingsgraad en juridisch statuut) gaat het precies?</t>
         </is>
       </c>
       <c r="B167" t="n">
         <v>0</v>
       </c>
       <c r="C167" t="n">
-        <v>0.9851678609848022</v>
+        <v>0.9898175597190857</v>
       </c>
       <c r="D167" t="n">
-        <v>0.01483213901519775</v>
+        <v>0.01018244028091431</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Zijn er in die context al overtredingen vastgesteld door en/of meldingen gemaakt bij de Onderwijsinspectie, de Vlaamse Ombudsdienst, het Kinderrechtencommissariaat of juridische instanties? Zo ja, om hoeveel klachten/meldingen gaat het hier?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal ongevallen met 6- tot 18-jarigen in andere provincies?</t>
         </is>
       </c>
       <c r="B168" t="n">
         <v>1</v>
       </c>
       <c r="C168" t="n">
-        <v>0.9855883717536926</v>
+        <v>0.9898236393928528</v>
       </c>
       <c r="D168" t="n">
-        <v>0.01441162824630737</v>
+        <v>0.01017636060714722</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Kan de minister een stand van zaken geven met betrekking tot deze uitvoering en de kosten?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal ongevallen met 6- tot 18-jarigen in andere provincies?</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C169" t="n">
-        <v>0.9856070280075073</v>
+        <v>0.9898236393928528</v>
       </c>
       <c r="D169" t="n">
-        <v>0.01439297199249268</v>
+        <v>0.01017636060714722</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Beschikt de minister over actuele cijfers met betrekking tot de langdurig zieken?</t>
+          <t>Hoe verhouden deze cijfers zich tot het aantal ongevallen met 6- tot 18-jarigen in andere provincies?</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170" t="n">
-        <v>0.9857675433158875</v>
+        <v>0.9898236393928528</v>
       </c>
       <c r="D170" t="n">
-        <v>0.01423245668411255</v>
+        <v>0.01017636060714722</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Maar in de eerste plaats wijzen ze op de urgente nood aan meer visie omtrent de opzet en de doelen van de B-stroom: wat moeten we in godsnaam met die grote groep 12- à 14-jarigen die zelfs na 6 jaar lager onderwijs niet meekunnen met die basis?</t>
+          <t>Zullen scholen vacante uren kunnen omzetten in een krediet om flexi-jobbers te kunnen betalen?</t>
         </is>
       </c>
       <c r="B171" t="n">
         <v>0</v>
       </c>
       <c r="C171" t="n">
-        <v>0.98593670129776</v>
+        <v>0.9900223612785339</v>
       </c>
       <c r="D171" t="n">
-        <v>0.01406329870223999</v>
+        <v>0.009977638721466064</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Zijn er nog andere manieren om als inburgeraar een vrijstelling te krijgen voor het luik kennis van het Nederlands? Zo ja, welke en hoe vaak werden die de voorbije vijf jaren gebruikt?</t>
+          <t>Hebben die geen gronden in bezit/gebruik (en dan verdwijnen er ook geen ha in de data als we die niet meetellen)?</t>
         </is>
       </c>
       <c r="B172" t="n">
         <v>0</v>
       </c>
       <c r="C172" t="n">
-        <v>0.9860836863517761</v>
+        <v>0.9901447296142578</v>
       </c>
       <c r="D172" t="n">
-        <v>0.01391631364822388</v>
+        <v>0.009855270385742188</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Wat was toen de evaluatie van de commissie over de proefopstelling en wat zijn de conclusies?</t>
+          <t>Welk gevolg werd er gegeven aan de dossiers?</t>
         </is>
       </c>
       <c r="B173" t="n">
         <v>0</v>
       </c>
       <c r="C173" t="n">
-        <v>0.9862408638000488</v>
+        <v>0.990577220916748</v>
       </c>
       <c r="D173" t="n">
-        <v>0.01375913619995117</v>
+        <v>0.009422779083251953</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>1 https://www.antigifcentrum.be/natuur/dieren/steken-van-wespen-bijen-hommels-en-aziatische-hoornaars2 https://natuurenbos.vlaanderen.be/schade-en-overlast/schade-overlast-door-invasieve-exoten/invasieve-exoten-vlaanderen 3 https://www.vespawatch.be/4 Wespennest gevonden?</t>
+          <t>a) Een overzicht van het aantal ondernemingen dat werkt met individueel maatwerkers, opgedeeld naar hoeveel individueel maatwerkers er actief zijn binnen de onderneming (ondernemingen met: minder dan 5, 5-10, 11-20, 21-50, 51-100, 100+).</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C174" t="n">
-        <v>0.9863090515136719</v>
+        <v>0.9906460046768188</v>
       </c>
       <c r="D174" t="n">
-        <v>0.01369094848632812</v>
+        <v>0.009353995323181152</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Kan een overzicht worden gegeven van de financiering van de aanpak van de knelpunten in de provincie Antwerpen?</t>
+          <t>b) Als blijkt dat er nog budget over is, wat zal de minister daar dan mee doen?</t>
         </is>
       </c>
       <c r="B175" t="n">
         <v>0</v>
       </c>
       <c r="C175" t="n">
-        <v>0.9863798022270203</v>
+        <v>0.9910049438476562</v>
       </c>
       <c r="D175" t="n">
-        <v>0.01362019777297974</v>
+        <v>0.00899505615234375</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>b) Ziet de minister een stijging of daling in die cijfers?</t>
+          <t>Deels?</t>
         </is>
       </c>
       <c r="B176" t="n">
         <v>0</v>
       </c>
       <c r="C176" t="n">
-        <v>0.9866151213645935</v>
+        <v>0.9910935759544373</v>
       </c>
       <c r="D176" t="n">
-        <v>0.01338487863540649</v>
+        <v>0.008906424045562744</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Kan de minister verduidelijken vanuit welk beleidsdomein die subsidiëring is gebeurd, of dat de financiering vanuit het Vlaamse Randfonds komt?</t>
+          <t>Is het gebruik van iPads en gsm’s achter het stuur wel toegestaan voor chauffeurs?</t>
         </is>
       </c>
       <c r="B177" t="n">
         <v>0</v>
       </c>
       <c r="C177" t="n">
-        <v>0.9866992235183716</v>
+        <v>0.9911508560180664</v>
       </c>
       <c r="D177" t="n">
-        <v>0.01330077648162842</v>
+        <v>0.008849143981933594</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>b) Is de geografische spreiding evenredig gebeurd of heeft men er bij de uiteindelijke selectie toch van afgeweken?</t>
+          <t>Beschikt de minister over de voornaamste reden van afwijzing?</t>
         </is>
       </c>
       <c r="B178" t="n">
         <v>0</v>
       </c>
       <c r="C178" t="n">
-        <v>0.9867645502090454</v>
+        <v>0.9912909269332886</v>
       </c>
       <c r="D178" t="n">
-        <v>0.01323544979095459</v>
+        <v>0.008709073066711426</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>b) Is de geografische spreiding evenredig gebeurd of heeft men er bij de uiteindelijke selectie toch van afgeweken?</t>
+          <t>Hoe lang worden ze al gebruikt?</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C179" t="n">
-        <v>0.9867645502090454</v>
+        <v>0.991445779800415</v>
       </c>
       <c r="D179" t="n">
-        <v>0.01323544979095459</v>
+        <v>0.008554220199584961</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Welke scholen in Vlaanderen werden uiteindelijk geselecteerd voor een auteursresidentie in het schooljaar 2023-2024?</t>
+          <t>In 2022, hoeveel sportwedstrijden en -competities werden rechtstreeks uitgezonden op de VRT?</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C180" t="n">
-        <v>0.9868266582489014</v>
+        <v>0.991814136505127</v>
       </c>
       <c r="D180" t="n">
-        <v>0.01317334175109863</v>
+        <v>0.008185863494873047</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Welke scholen in Vlaanderen werden uiteindelijk geselecteerd voor een auteursresidentie in het schooljaar 2023-2024?</t>
+          <t>STAGEbonussen in schooljaar 2021-2022?</t>
         </is>
       </c>
       <c r="B181" t="n">
         <v>0</v>
       </c>
       <c r="C181" t="n">
-        <v>0.9868266582489014</v>
+        <v>0.9918363690376282</v>
       </c>
       <c r="D181" t="n">
-        <v>0.01317334175109863</v>
+        <v>0.008163630962371826</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Als we in het basisonderwijs meteen al beginnen met sleutelcompetenties leeg te laten, dan zijn we toch een duidelijk signaal aan het geven dat niet alle sleutelcompetenties evenwaardig zijn en dat niet alle sleutelcompetenties belangrijk zijn?</t>
+          <t>Maakt die trajectcontrole langs de N368 effectief deel uit van de twintig nieuwe locaties die dit jaar door AWV werden geselecteerd?</t>
         </is>
       </c>
       <c r="B182" t="n">
         <v>0</v>
       </c>
       <c r="C182" t="n">
-        <v>0.9871658682823181</v>
+        <v>0.9919107556343079</v>
       </c>
       <c r="D182" t="n">
-        <v>0.01283413171768188</v>
+        <v>0.008089244365692139</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>d) Kan de minister ook een verder verloop en timing geven van het project?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met personenwagens en het aantal ingeschreven personenwagens, zonder de SUV’s?</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" t="n">
-        <v>0.9874371290206909</v>
+        <v>0.9922789335250854</v>
       </c>
       <c r="D183" t="n">
-        <v>0.01256287097930908</v>
+        <v>0.007721066474914551</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Hoe ver staat de voorstudie?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met personenwagens en het aantal ingeschreven personenwagens, zonder de SUV’s?</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C184" t="n">
-        <v>0.987558901309967</v>
+        <v>0.9922789335250854</v>
       </c>
       <c r="D184" t="n">
-        <v>0.01244109869003296</v>
+        <v>0.007721066474914551</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Hoe ver staat de voorstudie?</t>
+          <t>Kan de minister-president, meer specifiek voor het arrondissement Mechelen, een overzicht geven van de lokale straat-, buurt- of verenigingsinitiatieven die in 2023 en 2022 een feestcheque ontvingen?</t>
         </is>
       </c>
       <c r="B185" t="n">
         <v>0</v>
       </c>
       <c r="C185" t="n">
-        <v>0.987558901309967</v>
+        <v>0.9922996163368225</v>
       </c>
       <c r="D185" t="n">
-        <v>0.01244109869003296</v>
+        <v>0.00770038366317749</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Wordt er 1 miljoen euro bespaard op jeugdinfrastructuur?</t>
+          <t>e) Wordt voor het totaal van deze 674.000ha hectaresteun toegekend?</t>
         </is>
       </c>
       <c r="B186" t="n">
         <v>1</v>
       </c>
       <c r="C186" t="n">
-        <v>0.987754762172699</v>
+        <v>0.9923431277275085</v>
       </c>
       <c r="D186" t="n">
-        <v>0.01224523782730103</v>
+        <v>0.007656872272491455</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>- Voor welke mobiliteitshulpmiddelen is een tweedehandssysteem geschikt?</t>
+          <t>Worden in 2023 en 2024 specifieke acties opgezet op basis van wat men heeft geleerd uit de voorgaande jaren? Zo ja, welke en wat zijn de resultaten daarvan?</t>
         </is>
       </c>
       <c r="B187" t="n">
         <v>0</v>
       </c>
       <c r="C187" t="n">
-        <v>0.9877806901931763</v>
+        <v>0.9923507571220398</v>
       </c>
       <c r="D187" t="n">
-        <v>0.01221930980682373</v>
+        <v>0.007649242877960205</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Is de minister van oordeel dat er nood is aan meer en/of beter onderhouden openbare toiletten in de metrostations?</t>
+          <t>Graag verduidelijking over die extra 55-60.000ha:a) Onder welke categorieën worden deze gronden in het betaalorgaan genoteerd zodat ze daarna uit de cijfers kunnen gefilterd worden richting Statbel?</t>
         </is>
       </c>
       <c r="B188" t="n">
         <v>0</v>
       </c>
       <c r="C188" t="n">
-        <v>0.9878971576690674</v>
+        <v>0.9923515915870667</v>
       </c>
       <c r="D188" t="n">
-        <v>0.01210284233093262</v>
+        <v>0.00764840841293335</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Wat is het concrete doel van dat onderzoek?</t>
+          <t>2.Hoe en wanneer kan dit initiatief verder worden uitgerold over heel Vlaanderen ?</t>
         </is>
       </c>
       <c r="B189" t="n">
         <v>0</v>
       </c>
       <c r="C189" t="n">
-        <v>0.9879671931266785</v>
+        <v>0.9923552274703979</v>
       </c>
       <c r="D189" t="n">
-        <v>0.01203280687332153</v>
+        <v>0.007644772529602051</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Kan de minister een overzicht geven per West-Vlaamse gemeente van het huidige aantal kinderen in pleegzorg en het huidige aantal pleeggezinnen?</t>
+          <t>2.Hoe en wanneer kan dit initiatief verder worden uitgerold over heel Vlaanderen ?</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190" t="n">
-        <v>0.9881256818771362</v>
+        <v>0.9923552274703979</v>
       </c>
       <c r="D190" t="n">
-        <v>0.01187431812286377</v>
+        <v>0.007644772529602051</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Voldoet het museum aan de beoogde doelstellingen?</t>
+          <t>Wat was de kostprijs van de uitwerking van het ontwerp van de N41 door het studiebureau Tractebel Engineering nv?</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C191" t="n">
-        <v>0.9885184168815613</v>
+        <v>0.9924909472465515</v>
       </c>
       <c r="D191" t="n">
-        <v>0.01148158311843872</v>
+        <v>0.007509052753448486</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Voldoet het museum aan de beoogde doelstellingen?</t>
+          <t>Kan de minister een overzicht geven van het aantal verkeersslachtoffers bij 6- tot 18-jarigen die de laatste vijf jaar in Limburg vielen tijdens de uren van de verplaatsingen donderdag, vrijdag; 12-12.59u woensdag)?</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C192" t="n">
-        <v>0.9885184168815613</v>
+        <v>0.9926078319549561</v>
       </c>
       <c r="D192" t="n">
-        <v>0.01148158311843872</v>
+        <v>0.007392168045043945</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Voldoet het museum aan de beoogde doelstellingen?</t>
+          <t>Gebeurde er een vergelijking met andere systemen? Zo ja, welke en wat is het resultaat?</t>
         </is>
       </c>
       <c r="B193" t="n">
         <v>0</v>
       </c>
       <c r="C193" t="n">
-        <v>0.9885184168815613</v>
+        <v>0.9927772283554077</v>
       </c>
       <c r="D193" t="n">
-        <v>0.01148158311843872</v>
+        <v>0.007222771644592285</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Sinds wanneer ontvingen alle aanvragers deze informatie?</t>
+          <t>Beschikt de minister over de voornaamste redenen van afwijzing?</t>
         </is>
       </c>
       <c r="B194" t="n">
         <v>0</v>
       </c>
       <c r="C194" t="n">
-        <v>0.9885884523391724</v>
+        <v>0.9928029179573059</v>
       </c>
       <c r="D194" t="n">
-        <v>0.01141154766082764</v>
+        <v>0.007197082042694092</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Kan een overzicht gegeven worden van die knelpunten met opname van locatie en het probleem van het knelpunt?</t>
+          <t>Beschikt de minister over de voornaamste redenen van afwijzing?</t>
         </is>
       </c>
       <c r="B195" t="n">
         <v>0</v>
       </c>
       <c r="C195" t="n">
-        <v>0.988636314868927</v>
+        <v>0.9928029179573059</v>
       </c>
       <c r="D195" t="n">
-        <v>0.011363685131073</v>
+        <v>0.007197082042694092</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Kan de minister voor deze bestuursperiode meedelen op welke data hiervan gebruik werd gemaakt?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met SUV’s en het aantal ongevallen met andere personenwagens?</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C196" t="n">
-        <v>0.9887887835502625</v>
+        <v>0.9928814172744751</v>
       </c>
       <c r="D196" t="n">
-        <v>0.01121121644973755</v>
+        <v>0.007118582725524902</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Zijn ze veranderd doorheen de jaren?</t>
+          <t>Wat is de verhouding tussen het aantal ongevallen met SUV’s en het aantal ongevallen met andere personenwagens?</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C197" t="n">
-        <v>0.9888193011283875</v>
+        <v>0.9928814172744751</v>
       </c>
       <c r="D197" t="n">
-        <v>0.01118069887161255</v>
+        <v>0.007118582725524902</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Zijn ze veranderd doorheen de jaren?</t>
+          <t>Wat is het slaagpercentage van leerlingen die hun diploma secundair onderwijs via de centrale examencommissie wensen te behalen?</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C198" t="n">
-        <v>0.9888193011283875</v>
+        <v>0.9930777549743652</v>
       </c>
       <c r="D198" t="n">
-        <v>0.01118069887161255</v>
+        <v>0.006922245025634766</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Zijn ze veranderd doorheen de jaren?</t>
+          <t>Wat zal de minister doen om er voor te zorgen dat een Europees ambtenaar die zijn kind wil inschrijven in een kinderopvang van de Vlaamse Gemeenschap met inkomenstarief, de gepaste prijs betaalt op basis van zijn werkelijk nettoloon en werkelijke gezinssamenstelling?</t>
         </is>
       </c>
       <c r="B199" t="n">
         <v>0</v>
       </c>
       <c r="C199" t="n">
-        <v>0.9888193011283875</v>
+        <v>0.9932223558425903</v>
       </c>
       <c r="D199" t="n">
-        <v>0.01118069887161255</v>
+        <v>0.006777644157409668</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Moet de principiële stemming over de aankoop in de openbare of in de besloten vergadering plaatsvinden?</t>
+          <t>Wat waren die sancties per voorziening?</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C200" t="n">
-        <v>0.9889469742774963</v>
+        <v>0.993225634098053</v>
       </c>
       <c r="D200" t="n">
-        <v>0.01105302572250366</v>
+        <v>0.006774365901947021</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Kan de minister per dag tot en met 15 september het aantal inschrijvingen alsook het aantal aanvragen voor leerlingenvervoer meedelen?</t>
+          <t>Wat is de volledige kostprijs voor de aanpassingen die werden gedaan in de stelplaats Winterslag?</t>
         </is>
       </c>
       <c r="B201" t="n">
         <v>1</v>
       </c>
       <c r="C201" t="n">
-        <v>0.9890017509460449</v>
+        <v>0.9932437539100647</v>
       </c>
       <c r="D201" t="n">
-        <v>0.01099824905395508</v>
+        <v>0.006756246089935303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>